<commit_message>
get ModsRecord objects from DataHandler, instead of clients needing to know so much about the DataHandler class
</commit_message>
<xml_diff>
--- a/test_files/data.xlsx
+++ b/test_files/data.xlsx
@@ -1,23 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="161" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="161"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="70">
   <si>
     <t>Media Title</t>
   </si>
@@ -31,16 +35,16 @@
     <t>Orig. number</t>
   </si>
   <si>
-    <t>image_number </t>
-  </si>
-  <si>
-    <t>PN_DB_id </t>
+    <t>image_number</t>
+  </si>
+  <si>
+    <t>PN_DB_id</t>
   </si>
   <si>
     <t>OP and unit</t>
   </si>
   <si>
-    <t>long_caption </t>
+    <t>long_caption</t>
   </si>
   <si>
     <t>desc comp</t>
@@ -52,7 +56,7 @@
     <t>short_caption 2</t>
   </si>
   <si>
-    <t>date_added </t>
+    <t>date_added</t>
   </si>
   <si>
     <t>23-PN Index</t>
@@ -125,47 +129,47 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">&lt;mods:identifier type="local" displayLabel="Origin</t>
+      <t>&lt;mods:identifier type="local" displayLabel="Origin</t>
     </r>
     <r>
       <rPr>
+        <b/>
+        <sz val="10"/>
         <rFont val="DejaVu Sans"/>
+        <family val="2"/>
         <charset val="1"/>
-        <family val="2"/>
-        <b val="true"/>
-        <sz val="10"/>
       </rPr>
-      <t xml:space="preserve">ă</t>
+      <t>ă</t>
     </r>
     <r>
       <rPr>
+        <b/>
+        <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <charset val="1"/>
-        <family val="2"/>
-        <b val="true"/>
-        <sz val="10"/>
       </rPr>
-      <t xml:space="preserve">l no</t>
+      <t>l no</t>
     </r>
     <r>
       <rPr>
+        <b/>
+        <sz val="10"/>
         <rFont val="DejaVu Sans"/>
+        <family val="2"/>
         <charset val="1"/>
-        <family val="2"/>
-        <b val="true"/>
-        <sz val="10"/>
       </rPr>
-      <t xml:space="preserve">é</t>
+      <t>é</t>
     </r>
     <r>
       <rPr>
+        <b/>
+        <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <charset val="1"/>
-        <family val="2"/>
-        <b val="true"/>
-        <sz val="10"/>
       </rPr>
-      <t xml:space="preserve">."&gt;</t>
+      <t>."&gt;</t>
     </r>
   </si>
   <si>
@@ -245,9 +249,6 @@
   </si>
   <si>
     <t>random</t>
-  </si>
-  <si>
-    <t>test2</t>
   </si>
   <si>
     <t>Test 2</t>
@@ -277,76 +278,59 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="@" numFmtId="165"/>
-    <numFmt formatCode="YYYY\-MM\-DD" numFmtId="166"/>
-    <numFmt formatCode="M/D/YYYY" numFmtId="167"/>
-    <numFmt formatCode="DD/MM/YYYY" numFmtId="168"/>
-    <numFmt formatCode="#" numFmtId="169"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="167" formatCode="#"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <sz val="10"/>
     </font>
     <font>
+      <b/>
+      <sz val="10"/>
       <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
+      <b/>
       <sz val="10"/>
+      <name val="DejaVu Sans"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <name val="Arial"/>
+      <sz val="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <color rgb="00000000"/>
-      <sz val="10"/>
     </font>
     <font>
-      <name val="DejaVu Sans"/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="MS Sans Serif"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Verdana"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="MS Sans Serif"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <color rgb="00000000"/>
-      <sz val="8"/>
     </font>
   </fonts>
   <fills count="5">
@@ -358,188 +342,444 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00CCFFFF"/>
-        <bgColor rgb="00CCFFFF"/>
+        <fgColor rgb="FFCCFFFF"/>
+        <bgColor rgb="FFCCFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00CCFFCC"/>
-        <bgColor rgb="00CCFFFF"/>
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00C0C0C0"/>
-        <bgColor rgb="00CCCCFF"/>
+        <fgColor rgb="FFC0C0C0"/>
+        <bgColor rgb="FFCCCCFF"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="23">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="4" numFmtId="165" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="166" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="4" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="4" fontId="5" numFmtId="167" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="4" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="165" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="168" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="8" numFmtId="167" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="9" numFmtId="169" xfId="0">
-      <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="9" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="9" numFmtId="167" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="9" numFmtId="164" xfId="0">
-      <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG4"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D13" activeCellId="0" pane="topLeft" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6235294117647"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.6627450980392"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.5882352941176"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.3490196078431"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.7372549019608"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="53.5058823529412"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.4392156862745"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.9529411764706"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.6235294117647"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="29.6941176470588"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.6117647058824"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="73.2235294117647"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.6705882352941"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.6235294117647"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.2509803921569"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="28.2901960784314"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="29.1843137254902"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="34.4313725490196"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="21.4980392156863"/>
-    <col collapsed="false" hidden="false" max="21" min="20" style="0" width="11.6235294117647"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="46.4588235294118"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="37.6352941176471"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="14.9764705882353"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="17.9176470588235"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="16.2509803921569"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="32.3882352941176"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="39.4235294117647"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="13.8196078431373"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="18.5607843137255"/>
-    <col collapsed="false" hidden="false" max="32" min="31" style="0" width="11.6235294117647"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="13.0509803921569"/>
-    <col collapsed="false" hidden="false" max="1025" min="34" style="0" width="11.6235294117647"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="18.35" outlineLevel="0" r="1" s="9">
+    <row r="1" spans="1:33" s="9" customFormat="1" ht="18.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -640,7 +880,7 @@
         <v>32</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="19.85" outlineLevel="0" r="2" s="9">
+    <row r="2" spans="1:33" s="9" customFormat="1" ht="19.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>33</v>
       </c>
@@ -741,23 +981,23 @@
         <v>45</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="16.9" outlineLevel="0" r="3" s="14">
+    <row r="3" spans="1:33" s="14" customFormat="1" ht="17" customHeight="1">
       <c r="A3" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="10" t="n">
+      <c r="B3" s="10">
         <v>1</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="12" t="n">
+      <c r="D3" s="12">
         <v>123</v>
       </c>
-      <c r="E3" s="9" t="n">
+      <c r="E3" s="9">
         <v>12</v>
       </c>
-      <c r="F3" s="9" t="n">
+      <c r="F3" s="9">
         <v>12</v>
       </c>
       <c r="G3" s="13"/>
@@ -770,7 +1010,7 @@
       <c r="J3" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="L3" s="16" t="n">
+      <c r="L3" s="16">
         <v>38646</v>
       </c>
       <c r="M3" s="17" t="s">
@@ -779,7 +1019,7 @@
       <c r="N3" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="O3" s="18" t="n">
+      <c r="O3" s="18">
         <v>123</v>
       </c>
       <c r="P3" s="19" t="s">
@@ -799,7 +1039,7 @@
       <c r="V3" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="W3" s="20" t="n">
+      <c r="W3" s="20">
         <v>38635</v>
       </c>
       <c r="X3" s="19" t="s">
@@ -821,45 +1061,45 @@
       <c r="AF3" s="21"/>
       <c r="AG3" s="19"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="16.15" outlineLevel="0" r="4" s="14">
+    <row r="4" spans="1:33" s="14" customFormat="1" ht="16.25" customHeight="1">
       <c r="A4" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="10" t="n">
+      <c r="B4" s="10">
         <v>2</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="D4" s="12" t="n">
+        <v>48</v>
+      </c>
+      <c r="D4" s="12">
         <v>234</v>
       </c>
-      <c r="E4" s="9" t="n">
+      <c r="E4" s="9">
         <v>23</v>
       </c>
-      <c r="F4" s="9" t="n">
+      <c r="F4" s="9">
         <v>23</v>
       </c>
       <c r="G4" s="13"/>
       <c r="H4" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="I4" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="I4" s="15" t="s">
+      <c r="J4" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="L4" s="22">
+        <v>38646</v>
+      </c>
+      <c r="M4" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="N4" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="L4" s="22" t="n">
-        <v>38646</v>
-      </c>
-      <c r="M4" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="N4" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="O4" s="18" t="n">
+      <c r="O4" s="18">
         <v>234</v>
       </c>
       <c r="P4" s="19" t="s">
@@ -869,7 +1109,7 @@
         <v>54</v>
       </c>
       <c r="R4" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="S4" s="19"/>
       <c r="T4" s="19"/>
@@ -877,17 +1117,17 @@
         <v>56</v>
       </c>
       <c r="V4" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="W4" s="20" t="s">
         <v>68</v>
-      </c>
-      <c r="W4" s="20" t="s">
-        <v>69</v>
       </c>
       <c r="X4" s="19" t="s">
         <v>58</v>
       </c>
       <c r="Y4" s="19"/>
       <c r="Z4" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AA4" s="19" t="s">
         <v>60</v>
@@ -902,60 +1142,31 @@
       <c r="AG4" s="19"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG3"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C10" activeCellId="0" pane="topLeft" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6235294117647"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.3176470588235"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.5137254901961"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.4823529411765"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.9960784313725"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="52.5647058823529"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.6235294117647"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="27.4313725490196"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.3764705882353"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="29.5921568627451"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.6745098039216"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="72.4274509803922"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="11.6235294117647"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.3176470588235"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="27.8313725490196"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="28.2352941176471"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="33.9176470588235"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="21.6156862745098"/>
-    <col collapsed="false" hidden="false" max="21" min="20" style="0" width="11.6235294117647"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="46.7490196078431"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="37.5607843137255"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="14.9960784313725"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="19.5882352941177"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="18.6392156862745"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="31.7529411764706"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="39.0549019607843"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="15.1294117647059"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="18.7764705882353"/>
-    <col collapsed="false" hidden="false" max="1025" min="31" style="0" width="11.6235294117647"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="18.35" outlineLevel="0" r="1" s="9">
+    <row r="1" spans="1:33" s="9" customFormat="1" ht="18.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1056,7 +1267,7 @@
         <v>32</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="19.85" outlineLevel="0" r="2" s="9">
+    <row r="2" spans="1:33" s="9" customFormat="1" ht="19.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>33</v>
       </c>
@@ -1157,23 +1368,23 @@
         <v>45</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="16.9" outlineLevel="0" r="3" s="14">
+    <row r="3" spans="1:33" s="14" customFormat="1" ht="17" customHeight="1">
       <c r="A3" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="10" t="n">
+      <c r="B3" s="10">
         <v>1</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="12" t="n">
+      <c r="D3" s="12">
         <v>123</v>
       </c>
-      <c r="E3" s="9" t="n">
+      <c r="E3" s="9">
         <v>12</v>
       </c>
-      <c r="F3" s="9" t="n">
+      <c r="F3" s="9">
         <v>12</v>
       </c>
       <c r="G3" s="13"/>
@@ -1186,7 +1397,7 @@
       <c r="J3" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="L3" s="16" t="n">
+      <c r="L3" s="16">
         <v>39742</v>
       </c>
       <c r="M3" s="17" t="s">
@@ -1195,7 +1406,7 @@
       <c r="N3" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="O3" s="18" t="n">
+      <c r="O3" s="18">
         <v>123</v>
       </c>
       <c r="P3" s="19" t="s">
@@ -1215,7 +1426,7 @@
       <c r="V3" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="W3" s="20" t="n">
+      <c r="W3" s="20">
         <v>38635</v>
       </c>
       <c r="X3" s="19" t="s">
@@ -1238,37 +1449,38 @@
       <c r="AG3" s="19"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6235294117647"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>